<commit_message>
pushing results of augmentation
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WCDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9E41D0-792B-45F1-9949-052B6B72525B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72785240-6D6F-433E-B09F-869F452AEA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0BF925B6-910B-4B21-A80A-E5B412B92BF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="738" activeTab="9" xr2:uid="{0BF925B6-910B-4B21-A80A-E5B412B92BF7}"/>
   </bookViews>
   <sheets>
     <sheet name="TL" sheetId="10" r:id="rId1"/>
     <sheet name="FT" sheetId="11" r:id="rId2"/>
-    <sheet name="DenseNet121" sheetId="2" r:id="rId3"/>
-    <sheet name="MobileNetV2" sheetId="3" r:id="rId4"/>
-    <sheet name="VGG19" sheetId="4" r:id="rId5"/>
+    <sheet name="DenseNet121" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="MobileNetV2" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="VGG19" sheetId="4" state="hidden" r:id="rId5"/>
     <sheet name="AlexNet" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="InceptionV3" sheetId="9" r:id="rId7"/>
-    <sheet name="EfficientNetB1" sheetId="8" r:id="rId8"/>
+    <sheet name="InceptionV3" sheetId="9" state="hidden" r:id="rId7"/>
+    <sheet name="EfficientNetB1" sheetId="8" state="hidden" r:id="rId8"/>
     <sheet name="future_ideas" sheetId="12" r:id="rId9"/>
+    <sheet name="Data Extension" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="45">
   <si>
     <t>strategy</t>
   </si>
@@ -144,19 +145,63 @@
   </si>
   <si>
     <t>Give more weightatge to minor classses</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here I introduced more data in training_set for the minority classes </t>
+  </si>
+  <si>
+    <t>and trained the DenseNet121 Model</t>
+  </si>
+  <si>
+    <t>Finding</t>
+  </si>
+  <si>
+    <t>New data was added from kaggle wheat disease detection dataset and was labelled futher</t>
+  </si>
+  <si>
+    <t>Compared to original results, we actually see slight drops in the overall F1score values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I think this could be the due to the domain shift that might have happened. The distribution of dataset in my old training set might be different that the new one.</t>
+  </si>
+  <si>
+    <t>AFTER AUGMENTATION</t>
+  </si>
+  <si>
+    <t>shuffled</t>
+  </si>
+  <si>
+    <t>BEFORE AUGMENTATION</t>
+  </si>
+  <si>
+    <t>unshuffled train+valid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="6">
@@ -191,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -242,11 +287,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -291,15 +360,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -312,20 +372,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,20 +723,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67CBD9-02B7-47C2-97F9-376249E457A2}">
-  <dimension ref="B1:N18"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B3" sqref="B3:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -692,8 +774,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="2:14" ht="15" thickBot="1">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -730,8 +812,8 @@
         <v>63.24</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
+    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B5" s="22"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -747,7 +829,7 @@
       <c r="G5" s="9">
         <v>65.510000000000005</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -762,12 +844,12 @@
       <c r="M5" s="13">
         <v>71.510000000000005</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="17">
         <v>64.31</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="17"/>
+    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B6" s="23"/>
       <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
@@ -802,8 +884,8 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="23" t="s">
+    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B7" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -840,8 +922,8 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="24"/>
+    <row r="8" spans="2:14" ht="15" thickTop="1">
+      <c r="B8" s="22"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -876,8 +958,8 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="25"/>
+    <row r="9" spans="2:14" ht="15" thickBot="1">
+      <c r="B9" s="23"/>
       <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
@@ -890,12 +972,12 @@
       <c r="F9" s="13">
         <v>71.510000000000005</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="20">
         <v>64.31</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="2:14" ht="15" thickTop="1">
+      <c r="B10" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -914,8 +996,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
+    <row r="11" spans="2:14">
+      <c r="B11" s="22"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -932,8 +1014,8 @@
         <v>47.51</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="17"/>
+    <row r="12" spans="2:14" ht="15" thickBot="1">
+      <c r="B12" s="23"/>
       <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
@@ -950,8 +1032,8 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="2:14" ht="15" thickTop="1">
+      <c r="B13" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -970,8 +1052,8 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
+    <row r="14" spans="2:14">
+      <c r="B14" s="22"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -988,8 +1070,8 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="17"/>
+    <row r="15" spans="2:14" ht="15" thickBot="1">
+      <c r="B15" s="23"/>
       <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1006,8 +1088,8 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+    <row r="16" spans="2:14" ht="15" thickTop="1">
+      <c r="B16" s="24" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1026,8 +1108,8 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
+    <row r="17" spans="1:7">
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1044,8 +1126,8 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
+    <row r="18" spans="1:7">
+      <c r="B18" s="22"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1060,6 +1142,43 @@
       </c>
       <c r="G18" s="9">
         <v>23.37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1074,22 +1193,446 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1249699-A01A-4CFB-9DA3-BFA122B0A4C5}">
+  <dimension ref="B2:U39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="5.44140625" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9">
+        <v>15.21</v>
+      </c>
+      <c r="E6" s="9">
+        <v>92.8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>81.05</v>
+      </c>
+      <c r="G6" s="9">
+        <v>77.33</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>13.68</v>
+      </c>
+      <c r="K6" s="4">
+        <v>92.48</v>
+      </c>
+      <c r="L6" s="4">
+        <v>80.22</v>
+      </c>
+      <c r="M6" s="4">
+        <v>78.92</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="4">
+        <v>14.57</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>91.95</v>
+      </c>
+      <c r="R6" s="4">
+        <v>80.61</v>
+      </c>
+      <c r="S6" s="4">
+        <v>78.56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="22"/>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9">
+        <v>22.48</v>
+      </c>
+      <c r="E7" s="9">
+        <v>83.61</v>
+      </c>
+      <c r="F7" s="9">
+        <v>67.180000000000007</v>
+      </c>
+      <c r="G7" s="9">
+        <v>65.510000000000005</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="4">
+        <v>23.93</v>
+      </c>
+      <c r="K7" s="4">
+        <v>80.989999999999995</v>
+      </c>
+      <c r="L7" s="4">
+        <v>62.6</v>
+      </c>
+      <c r="M7" s="4">
+        <v>62.04</v>
+      </c>
+      <c r="O7" s="29"/>
+      <c r="P7" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>89.81</v>
+      </c>
+      <c r="R7" s="4">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="S7" s="4">
+        <v>77.319999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="15" thickBot="1">
+      <c r="B8" s="23"/>
+      <c r="C8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13">
+        <v>23.41</v>
+      </c>
+      <c r="E8" s="13">
+        <v>81.09</v>
+      </c>
+      <c r="F8" s="13">
+        <v>68.069999999999993</v>
+      </c>
+      <c r="G8" s="13">
+        <v>63.24</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" s="4">
+        <v>24.93</v>
+      </c>
+      <c r="K8" s="4">
+        <v>79.62</v>
+      </c>
+      <c r="L8" s="4">
+        <v>63.48</v>
+      </c>
+      <c r="M8" s="4">
+        <v>60.24</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="4">
+        <v>23.11</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>79.41</v>
+      </c>
+      <c r="R8" s="4">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="S8" s="4">
+        <v>63.88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="15" thickTop="1"/>
+    <row r="11" spans="2:19">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5.8</v>
+      </c>
+      <c r="E13" s="9">
+        <v>96.34</v>
+      </c>
+      <c r="F13" s="9">
+        <v>95.24</v>
+      </c>
+      <c r="G13" s="9">
+        <v>84.78</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>6.74</v>
+      </c>
+      <c r="K13" s="4">
+        <v>96.42</v>
+      </c>
+      <c r="L13" s="4">
+        <v>93.12</v>
+      </c>
+      <c r="M13" s="4">
+        <v>86.61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="B14" s="22"/>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9">
+        <v>18.86</v>
+      </c>
+      <c r="E14" s="9">
+        <v>83.88</v>
+      </c>
+      <c r="F14" s="9">
+        <v>77.48</v>
+      </c>
+      <c r="G14" s="9">
+        <v>69.849999999999994</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="4">
+        <v>20.29</v>
+      </c>
+      <c r="K14" s="4">
+        <v>82.05</v>
+      </c>
+      <c r="L14" s="4">
+        <v>73.28</v>
+      </c>
+      <c r="M14" s="4">
+        <v>67.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="22"/>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="9">
+        <v>18.25</v>
+      </c>
+      <c r="E15" s="9">
+        <v>82.24</v>
+      </c>
+      <c r="F15" s="9">
+        <v>78.78</v>
+      </c>
+      <c r="G15" s="21">
+        <v>71.38</v>
+      </c>
+      <c r="I15" s="24"/>
+      <c r="J15" s="4">
+        <v>19.72</v>
+      </c>
+      <c r="K15" s="4">
+        <v>81.25</v>
+      </c>
+      <c r="L15" s="4">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="M15" s="4">
+        <v>66.02</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21">
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+    </row>
+    <row r="18" spans="2:21">
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+    </row>
+    <row r="28" spans="2:21">
+      <c r="B28" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B13:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBA9A2A-1254-4B88-9610-852D86DB7252}">
-  <dimension ref="B1:N22"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1127,8 +1670,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="2:14">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1146,7 +1689,7 @@
       <c r="G4" s="9">
         <v>84.78</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -1161,12 +1704,12 @@
       <c r="M4" s="9">
         <v>78.78</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="16">
         <v>71.38</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="24"/>
+    <row r="5" spans="2:14">
+      <c r="B5" s="22"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1182,7 +1725,7 @@
       <c r="G5" s="9">
         <v>69.849999999999994</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="18" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -1197,12 +1740,12 @@
       <c r="M5" s="9">
         <v>75.91</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="16">
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
+    <row r="6" spans="2:14">
+      <c r="B6" s="22"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1758,7 @@
       <c r="F6" s="9">
         <v>78.78</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="21">
         <v>71.38</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -1237,8 +1780,8 @@
         <v>62.61</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="2:14">
+      <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1275,8 +1818,8 @@
         <v>63.17</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
+    <row r="8" spans="2:14">
+      <c r="B8" s="22"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1311,8 +1854,8 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
+    <row r="9" spans="2:14">
+      <c r="B9" s="22"/>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1325,12 +1868,12 @@
       <c r="F9" s="9">
         <v>75.91</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="21">
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="2:14">
+      <c r="B10" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1349,8 +1892,8 @@
         <v>80.44</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
+    <row r="11" spans="2:14">
+      <c r="B11" s="22"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1367,8 +1910,8 @@
         <v>63.71</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
+    <row r="12" spans="2:14">
+      <c r="B12" s="22"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1385,8 +1928,8 @@
         <v>62.61</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+    <row r="13" spans="2:14">
+      <c r="B13" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1405,8 +1948,8 @@
         <v>86.06</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
+    <row r="14" spans="2:14">
+      <c r="B14" s="22"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1423,8 +1966,8 @@
         <v>66.23</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
+    <row r="15" spans="2:14">
+      <c r="B15" s="22"/>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1440,9 +1983,22 @@
       <c r="G15" s="9">
         <v>63.17</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="J15" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" s="25"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1460,9 +2016,24 @@
       <c r="G16" s="9">
         <v>23.58</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
+      <c r="J16" s="26">
+        <v>0</v>
+      </c>
+      <c r="K16" s="27">
+        <v>6.74</v>
+      </c>
+      <c r="L16" s="27">
+        <v>96.42</v>
+      </c>
+      <c r="M16" s="27">
+        <v>93.12</v>
+      </c>
+      <c r="N16" s="27">
+        <v>86.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1478,9 +2049,24 @@
       <c r="G17" s="9">
         <v>23.64</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
+      <c r="J17" s="26">
+        <v>1</v>
+      </c>
+      <c r="K17" s="27">
+        <v>20.29</v>
+      </c>
+      <c r="L17" s="27">
+        <v>82.05</v>
+      </c>
+      <c r="M17" s="27">
+        <v>73.28</v>
+      </c>
+      <c r="N17" s="27">
+        <v>67.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="B18" s="22"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1496,8 +2082,44 @@
       <c r="G18" s="9">
         <v>23.37</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="J18" s="26">
+        <v>2</v>
+      </c>
+      <c r="K18" s="27">
+        <v>19.72</v>
+      </c>
+      <c r="L18" s="27">
+        <v>81.25</v>
+      </c>
+      <c r="M18" s="27">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="N18" s="27">
+        <v>66.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1"/>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B4:B6"/>
@@ -1518,7 +2140,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -1529,12 +2151,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +2179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1580,7 +2202,7 @@
         <v>77.33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +2225,7 @@
         <v>65.510000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1626,12 +2248,12 @@
         <v>63.24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +2276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1677,7 +2299,7 @@
         <v>84.78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -1694,7 +2316,7 @@
         <v>69.849999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1721,10 +2343,10 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -1735,12 +2357,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1763,7 +2385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1786,7 +2408,7 @@
         <v>84.84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +2431,7 @@
         <v>65.08</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1832,12 +2454,12 @@
         <v>64.31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1860,7 +2482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1883,7 +2505,7 @@
         <v>86.46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -1900,7 +2522,7 @@
         <v>67.459999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1927,10 +2549,10 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -1941,12 +2563,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1969,7 +2591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1992,7 +2614,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2637,7 @@
         <v>47.51</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2038,12 +2660,12 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2066,7 +2688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2089,7 +2711,7 @@
         <v>80.44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2106,7 +2728,7 @@
         <v>63.71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2136,7 +2758,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2147,12 +2769,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2175,7 +2797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2812,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2827,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2220,12 +2842,12 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2263,7 +2885,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2272,7 +2894,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2291,17 +2913,17 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2324,7 +2946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2347,7 +2969,7 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2370,7 +2992,7 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2393,12 +3015,12 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +3043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2444,7 +3066,7 @@
         <v>86.06</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2461,7 +3083,7 @@
         <v>66.23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2488,10 +3110,10 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2502,12 +3124,12 @@
     <col min="8" max="8" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2530,7 +3152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2553,7 +3175,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2576,7 +3198,7 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2599,12 +3221,12 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2627,7 +3249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2650,7 +3272,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2667,7 +3289,7 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2694,25 +3316,25 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B27" sqref="B26:B27"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -2720,7 +3342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +3350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -2736,7 +3358,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
adding results and code for data extension trial
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WCDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72785240-6D6F-433E-B09F-869F452AEA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC291CC-1F8F-4984-9FE9-A48B5ED3F750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="738" activeTab="9" xr2:uid="{0BF925B6-910B-4B21-A80A-E5B412B92BF7}"/>
   </bookViews>
@@ -21,8 +21,9 @@
     <sheet name="AlexNet" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="InceptionV3" sheetId="9" state="hidden" r:id="rId7"/>
     <sheet name="EfficientNetB1" sheetId="8" state="hidden" r:id="rId8"/>
-    <sheet name="future_ideas" sheetId="12" r:id="rId9"/>
-    <sheet name="Data Extension" sheetId="13" r:id="rId10"/>
+    <sheet name="Data Extension" sheetId="13" r:id="rId9"/>
+    <sheet name="Data Extension+augmentations" sheetId="14" r:id="rId10"/>
+    <sheet name="future_ideas" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="49">
   <si>
     <t>strategy</t>
   </si>
@@ -178,6 +179,18 @@
   </si>
   <si>
     <t>unshuffled train+valid</t>
+  </si>
+  <si>
+    <t>There is a domain shift problem</t>
+  </si>
+  <si>
+    <t>original dataset</t>
+  </si>
+  <si>
+    <t>dataset after adding new examples for minority classes</t>
+  </si>
+  <si>
+    <t>dynamically apply online augmentation to kaggle dataset and see the results</t>
   </si>
 </sst>
 </file>
@@ -204,7 +217,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -378,6 +397,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,27 +419,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,7 +767,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
@@ -775,7 +816,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -813,7 +854,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B5" s="22"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -849,7 +890,7 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B6" s="23"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
@@ -885,7 +926,7 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -923,7 +964,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickTop="1">
-      <c r="B8" s="22"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -959,7 +1000,7 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1">
-      <c r="B9" s="23"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
@@ -977,7 +1018,7 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickTop="1">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -997,7 +1038,7 @@
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="22"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1056,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1">
-      <c r="B12" s="23"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1074,7 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickTop="1">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1053,7 +1094,7 @@
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="22"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1071,7 +1112,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" thickBot="1">
-      <c r="B15" s="23"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1089,7 +1130,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickTop="1">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1109,7 +1150,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="22"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1127,7 +1168,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="22"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1194,11 +1235,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1249699-A01A-4CFB-9DA3-BFA122B0A4C5}">
-  <dimension ref="B2:U39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B198147-95F5-407D-95B2-06BC79801C34}">
+  <dimension ref="B2:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4"/>
@@ -1207,7 +1248,7 @@
     <col min="14" max="14" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19">
+    <row r="2" spans="2:14">
       <c r="B2" t="s">
         <v>43</v>
       </c>
@@ -1215,18 +1256,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19">
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+    </row>
+    <row r="5" spans="2:14">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1245,39 +1286,25 @@
       <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19">
-      <c r="B6" s="22" t="s">
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1295,39 +1322,17 @@
       <c r="G6" s="9">
         <v>77.33</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="4">
-        <v>13.68</v>
-      </c>
-      <c r="K6" s="4">
-        <v>92.48</v>
-      </c>
-      <c r="L6" s="4">
-        <v>80.22</v>
-      </c>
-      <c r="M6" s="4">
-        <v>78.92</v>
-      </c>
-      <c r="O6" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P6" s="4">
-        <v>14.57</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>91.95</v>
-      </c>
-      <c r="R6" s="4">
-        <v>80.61</v>
-      </c>
-      <c r="S6" s="4">
-        <v>78.56</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19">
-      <c r="B7" s="22"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="30"/>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="27"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1343,35 +1348,15 @@
       <c r="G7" s="9">
         <v>65.510000000000005</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="4">
-        <v>23.93</v>
-      </c>
-      <c r="K7" s="4">
-        <v>80.989999999999995</v>
-      </c>
-      <c r="L7" s="4">
-        <v>62.6</v>
-      </c>
-      <c r="M7" s="4">
-        <v>62.04</v>
-      </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="4">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>89.81</v>
-      </c>
-      <c r="R7" s="4">
-        <v>77.540000000000006</v>
-      </c>
-      <c r="S7" s="4">
-        <v>77.319999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" ht="15" thickBot="1">
-      <c r="B8" s="23"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="2:14" ht="15" thickBot="1">
+      <c r="B8" s="28"/>
       <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
@@ -1387,40 +1372,41 @@
       <c r="G8" s="13">
         <v>63.24</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4">
-        <v>24.93</v>
-      </c>
-      <c r="K8" s="4">
-        <v>79.62</v>
-      </c>
-      <c r="L8" s="4">
-        <v>63.48</v>
-      </c>
-      <c r="M8" s="4">
-        <v>60.24</v>
-      </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="4">
-        <v>23.11</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>79.41</v>
-      </c>
-      <c r="R8" s="4">
-        <v>66.349999999999994</v>
-      </c>
-      <c r="S8" s="4">
-        <v>63.88</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" ht="15" thickTop="1"/>
-    <row r="11" spans="2:19">
+      <c r="I8" s="35"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="30"/>
+    </row>
+    <row r="9" spans="2:14" ht="15" thickTop="1">
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="2:14">
       <c r="B11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:19">
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
@@ -1439,24 +1425,25 @@
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:19">
-      <c r="B13" s="22" t="s">
+      <c r="N12" s="30"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1474,24 +1461,17 @@
       <c r="G13" s="9">
         <v>84.78</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="4">
-        <v>6.74</v>
-      </c>
-      <c r="K13" s="4">
-        <v>96.42</v>
-      </c>
-      <c r="L13" s="4">
-        <v>93.12</v>
-      </c>
-      <c r="M13" s="4">
-        <v>86.61</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19">
-      <c r="B14" s="22"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="30"/>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="27"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1507,22 +1487,15 @@
       <c r="G14" s="9">
         <v>69.849999999999994</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="4">
-        <v>20.29</v>
-      </c>
-      <c r="K14" s="4">
-        <v>82.05</v>
-      </c>
-      <c r="L14" s="4">
-        <v>73.28</v>
-      </c>
-      <c r="M14" s="4">
-        <v>67.25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19">
-      <c r="B15" s="22"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="30"/>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="27"/>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1538,44 +1511,48 @@
       <c r="G15" s="21">
         <v>71.38</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="4">
-        <v>19.72</v>
-      </c>
-      <c r="K15" s="4">
-        <v>81.25</v>
-      </c>
-      <c r="L15" s="4">
-        <v>74.569999999999993</v>
-      </c>
-      <c r="M15" s="4">
-        <v>66.02</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21">
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-    </row>
-    <row r="18" spans="2:21">
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-    </row>
-    <row r="28" spans="2:21">
-      <c r="B28" s="31" t="s">
+      <c r="I15" s="35"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="30"/>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="C18" s="40"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:21">
+    <row r="29" spans="2:16">
       <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="2:16">
       <c r="B30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:21">
+    <row r="31" spans="2:16">
       <c r="B31" t="s">
         <v>38</v>
       </c>
@@ -1586,33 +1563,92 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="B6:B8"/>
     <mergeCell ref="I6:I8"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="I13:I15"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966EE664-FBF6-4CD7-8C19-21757BCFFEB1}">
+  <dimension ref="B3:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="M14:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1671,7 +1707,7 @@
       </c>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1709,7 +1745,7 @@
       </c>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="22"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1745,7 +1781,7 @@
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="22"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1781,7 +1817,7 @@
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1819,7 +1855,7 @@
       </c>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="22"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1855,7 +1891,7 @@
       </c>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="22"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1873,7 +1909,7 @@
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1893,7 +1929,7 @@
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="22"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1911,7 +1947,7 @@
       </c>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="22"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1929,7 +1965,7 @@
       </c>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1949,7 +1985,7 @@
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="22"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1967,7 +2003,7 @@
       </c>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="22"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1983,22 +2019,22 @@
       <c r="G15" s="9">
         <v>63.17</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="26" t="s">
+      <c r="L15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="26" t="s">
+      <c r="M15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N15" s="25"/>
+      <c r="N15" s="22"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2016,24 +2052,24 @@
       <c r="G16" s="9">
         <v>23.58</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="23">
         <v>0</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="24">
         <v>6.74</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="24">
         <v>96.42</v>
       </c>
-      <c r="M16" s="27">
+      <c r="M16" s="24">
         <v>93.12</v>
       </c>
-      <c r="N16" s="27">
+      <c r="N16" s="24">
         <v>86.61</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="B17" s="22"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2049,24 +2085,24 @@
       <c r="G17" s="9">
         <v>23.64</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="23">
         <v>1</v>
       </c>
-      <c r="K17" s="27">
+      <c r="K17" s="24">
         <v>20.29</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L17" s="24">
         <v>82.05</v>
       </c>
-      <c r="M17" s="27">
+      <c r="M17" s="24">
         <v>73.28</v>
       </c>
-      <c r="N17" s="27">
+      <c r="N17" s="24">
         <v>67.25</v>
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="B18" s="22"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2082,19 +2118,19 @@
       <c r="G18" s="9">
         <v>23.37</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="23">
         <v>2</v>
       </c>
-      <c r="K18" s="27">
+      <c r="K18" s="24">
         <v>19.72</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="24">
         <v>81.25</v>
       </c>
-      <c r="M18" s="27">
+      <c r="M18" s="24">
         <v>74.569999999999993</v>
       </c>
-      <c r="N18" s="27">
+      <c r="N18" s="24">
         <v>66.02</v>
       </c>
     </row>
@@ -3312,61 +3348,538 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966EE664-FBF6-4CD7-8C19-21757BCFFEB1}">
-  <dimension ref="B3:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1249699-A01A-4CFB-9DA3-BFA122B0A4C5}">
+  <dimension ref="B2:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
+    <row r="2" spans="2:19">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="30"/>
+      <c r="O5" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9">
+        <v>15.21</v>
+      </c>
+      <c r="E6" s="9">
+        <v>92.8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>81.05</v>
+      </c>
+      <c r="G6" s="9">
+        <v>77.33</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="33">
+        <v>14.57</v>
+      </c>
+      <c r="K6" s="33">
+        <v>91.95</v>
+      </c>
+      <c r="L6" s="33">
+        <v>80.61</v>
+      </c>
+      <c r="M6" s="33">
+        <v>78.56</v>
+      </c>
+      <c r="N6" s="30"/>
+      <c r="O6" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="36">
+        <v>13.68</v>
+      </c>
+      <c r="Q6" s="36">
+        <v>92.48</v>
+      </c>
+      <c r="R6" s="36">
+        <v>80.22</v>
+      </c>
+      <c r="S6" s="36">
+        <v>78.92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="27"/>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9">
+        <v>22.48</v>
+      </c>
+      <c r="E7" s="9">
+        <v>83.61</v>
+      </c>
+      <c r="F7" s="9">
+        <v>67.180000000000007</v>
+      </c>
+      <c r="G7" s="9">
+        <v>65.510000000000005</v>
+      </c>
+      <c r="I7" s="34"/>
+      <c r="J7" s="33">
+        <v>16</v>
+      </c>
+      <c r="K7" s="33">
+        <v>89.81</v>
+      </c>
+      <c r="L7" s="33">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="M7" s="33">
+        <v>77.319999999999993</v>
+      </c>
+      <c r="N7" s="30"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="36">
+        <v>23.93</v>
+      </c>
+      <c r="Q7" s="36">
+        <v>80.989999999999995</v>
+      </c>
+      <c r="R7" s="36">
+        <v>62.6</v>
+      </c>
+      <c r="S7" s="36">
+        <v>62.04</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="15" thickBot="1">
+      <c r="B8" s="28"/>
+      <c r="C8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13">
+        <v>23.41</v>
+      </c>
+      <c r="E8" s="13">
+        <v>81.09</v>
+      </c>
+      <c r="F8" s="13">
+        <v>68.069999999999993</v>
+      </c>
+      <c r="G8" s="13">
+        <v>63.24</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="33">
+        <v>23.11</v>
+      </c>
+      <c r="K8" s="33">
+        <v>79.41</v>
+      </c>
+      <c r="L8" s="33">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="M8" s="33">
+        <v>63.88</v>
+      </c>
+      <c r="N8" s="30"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="36">
+        <v>24.93</v>
+      </c>
+      <c r="Q8" s="36">
+        <v>79.62</v>
+      </c>
+      <c r="R8" s="36">
+        <v>63.48</v>
+      </c>
+      <c r="S8" s="36">
+        <v>60.24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="15" thickTop="1">
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+    </row>
+    <row r="11" spans="2:19">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="30"/>
+      <c r="O12" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5.8</v>
+      </c>
+      <c r="E13" s="9">
+        <v>96.34</v>
+      </c>
+      <c r="F13" s="9">
+        <v>95.24</v>
+      </c>
+      <c r="G13" s="9">
+        <v>84.78</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="33">
+        <v>7.99</v>
+      </c>
+      <c r="K13" s="33">
+        <v>95.24</v>
+      </c>
+      <c r="L13" s="33">
+        <v>90.84</v>
+      </c>
+      <c r="M13" s="33">
+        <v>84.77</v>
+      </c>
+      <c r="N13" s="30"/>
+      <c r="O13" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="36">
+        <v>6.74</v>
+      </c>
+      <c r="Q13" s="36">
+        <v>96.42</v>
+      </c>
+      <c r="R13" s="36">
+        <v>93.12</v>
+      </c>
+      <c r="S13" s="36">
+        <v>86.61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="B14" s="27"/>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9">
+        <v>18.86</v>
+      </c>
+      <c r="E14" s="9">
+        <v>83.88</v>
+      </c>
+      <c r="F14" s="9">
+        <v>77.48</v>
+      </c>
+      <c r="G14" s="9">
+        <v>69.849999999999994</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="33">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="K14" s="33">
+        <v>92.72</v>
+      </c>
+      <c r="L14" s="33">
+        <v>88.98</v>
+      </c>
+      <c r="M14" s="33">
+        <v>82.47</v>
+      </c>
+      <c r="N14" s="30"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="36">
+        <v>20.29</v>
+      </c>
+      <c r="Q14" s="36">
+        <v>82.05</v>
+      </c>
+      <c r="R14" s="36">
+        <v>73.28</v>
+      </c>
+      <c r="S14" s="36">
+        <v>67.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="27"/>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="9">
+        <v>18.25</v>
+      </c>
+      <c r="E15" s="9">
+        <v>82.24</v>
+      </c>
+      <c r="F15" s="9">
+        <v>78.78</v>
+      </c>
+      <c r="G15" s="21">
+        <v>71.38</v>
+      </c>
+      <c r="I15" s="35"/>
+      <c r="J15" s="33">
+        <v>18.48</v>
+      </c>
+      <c r="K15" s="33">
+        <v>82.77</v>
+      </c>
+      <c r="L15" s="33">
+        <v>74.38</v>
+      </c>
+      <c r="M15" s="33">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="N15" s="30"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="36">
+        <v>19.72</v>
+      </c>
+      <c r="Q15" s="36">
+        <v>81.25</v>
+      </c>
+      <c r="R15" s="36">
+        <v>74.569999999999993</v>
+      </c>
+      <c r="S15" s="36">
+        <v>66.02</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21">
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+    </row>
+    <row r="18" spans="2:21">
+      <c r="C18" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+    </row>
+    <row r="28" spans="2:21">
+      <c r="B28" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="O13:O15"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="I13:I15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added results with data aug
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WCDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC291CC-1F8F-4984-9FE9-A48B5ED3F750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B7B716-56B9-4E76-B88B-BBE3CA92EA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="738" activeTab="9" xr2:uid="{0BF925B6-910B-4B21-A80A-E5B412B92BF7}"/>
   </bookViews>
@@ -21,8 +21,8 @@
     <sheet name="AlexNet" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="InceptionV3" sheetId="9" state="hidden" r:id="rId7"/>
     <sheet name="EfficientNetB1" sheetId="8" state="hidden" r:id="rId8"/>
-    <sheet name="Data Extension" sheetId="13" r:id="rId9"/>
-    <sheet name="Data Extension+augmentations" sheetId="14" r:id="rId10"/>
+    <sheet name="balanced labels" sheetId="13" r:id="rId9"/>
+    <sheet name="Data balance+augmentations" sheetId="14" r:id="rId10"/>
     <sheet name="future_ideas" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="50">
   <si>
     <t>strategy</t>
   </si>
@@ -169,15 +169,9 @@
     <t xml:space="preserve"> I think this could be the due to the domain shift that might have happened. The distribution of dataset in my old training set might be different that the new one.</t>
   </si>
   <si>
-    <t>AFTER AUGMENTATION</t>
-  </si>
-  <si>
     <t>shuffled</t>
   </si>
   <si>
-    <t>BEFORE AUGMENTATION</t>
-  </si>
-  <si>
     <t>unshuffled train+valid</t>
   </si>
   <si>
@@ -190,31 +184,29 @@
     <t>dataset after adding new examples for minority classes</t>
   </si>
   <si>
-    <t>dynamically apply online augmentation to kaggle dataset and see the results</t>
+    <t>balanced data with augmentations</t>
+  </si>
+  <si>
+    <t>balanced data without augmentations</t>
+  </si>
+  <si>
+    <t>Original data with label imbalancing</t>
+  </si>
+  <si>
+    <t>dynamically apply light augmentation to external dataset and see the results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="7">
@@ -255,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -330,6 +322,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -379,14 +386,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -397,18 +398,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,35 +422,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,17 +776,17 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -815,8 +824,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1">
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -853,8 +862,8 @@
         <v>63.24</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B5" s="27"/>
+    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="25"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -870,7 +879,7 @@
       <c r="G5" s="9">
         <v>65.510000000000005</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -885,12 +894,12 @@
       <c r="M5" s="13">
         <v>71.510000000000005</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="16">
         <v>64.31</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B6" s="28"/>
+    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="26"/>
       <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
@@ -925,8 +934,8 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B7" s="29" t="s">
+    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -963,8 +972,8 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15" thickTop="1">
-      <c r="B8" s="27"/>
+    <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -999,8 +1008,8 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1">
-      <c r="B9" s="28"/>
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="26"/>
       <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
@@ -1013,12 +1022,12 @@
       <c r="F9" s="13">
         <v>71.510000000000005</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="18">
         <v>64.31</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15" thickTop="1">
-      <c r="B10" s="29" t="s">
+    <row r="10" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1037,8 +1046,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="27"/>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1055,8 +1064,8 @@
         <v>47.51</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1">
-      <c r="B12" s="28"/>
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="26"/>
       <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1073,8 +1082,8 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15" thickTop="1">
-      <c r="B13" s="29" t="s">
+    <row r="13" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1093,8 +1102,8 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="27"/>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1111,8 +1120,8 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1">
-      <c r="B15" s="28"/>
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="26"/>
       <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1129,8 +1138,8 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15" thickTop="1">
-      <c r="B16" s="29" t="s">
+    <row r="16" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1149,8 +1158,8 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="B17" s="27"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1167,8 +1176,8 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="27"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="25"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1185,12 +1194,12 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1236,38 +1245,36 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B198147-95F5-407D-95B2-06BC79801C34}">
-  <dimension ref="B2:P39"/>
+  <dimension ref="B2:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="5.44140625" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-    </row>
-    <row r="5" spans="2:14">
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1286,25 +1293,39 @@
       <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="J5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="K5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="L5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="M5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="N5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="30"/>
-    </row>
-    <row r="6" spans="2:14">
-      <c r="B6" s="27" t="s">
+      <c r="P5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1322,17 +1343,40 @@
       <c r="G6" s="9">
         <v>77.33</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="J6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="30"/>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="B7" s="27"/>
+      <c r="K6" s="4">
+        <v>14.57</v>
+      </c>
+      <c r="L6" s="4">
+        <v>91.95</v>
+      </c>
+      <c r="M6" s="4">
+        <v>80.61</v>
+      </c>
+      <c r="N6" s="4">
+        <v>78.56</v>
+      </c>
+      <c r="O6" s="21"/>
+      <c r="P6" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>17</v>
+      </c>
+      <c r="R6" s="4">
+        <v>90.68</v>
+      </c>
+      <c r="S6" s="4">
+        <v>78.69</v>
+      </c>
+      <c r="T6" s="4">
+        <v>77.08</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1348,15 +1392,36 @@
       <c r="G7" s="9">
         <v>65.510000000000005</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="30"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1">
-      <c r="B8" s="28"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="4">
+        <v>16</v>
+      </c>
+      <c r="L7" s="4">
+        <v>89.81</v>
+      </c>
+      <c r="M7" s="4">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="N7" s="4">
+        <v>77.319999999999993</v>
+      </c>
+      <c r="O7" s="21"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="4">
+        <v>17.87</v>
+      </c>
+      <c r="R7" s="4">
+        <v>87.91</v>
+      </c>
+      <c r="S7" s="4">
+        <v>76.89</v>
+      </c>
+      <c r="T7" s="4">
+        <v>75.459999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="26"/>
       <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
@@ -1372,41 +1437,41 @@
       <c r="G8" s="13">
         <v>63.24</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="30"/>
-    </row>
-    <row r="9" spans="2:14" ht="15" thickTop="1">
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="J8" s="27"/>
+      <c r="K8" s="4">
+        <v>23.11</v>
+      </c>
+      <c r="L8" s="4">
+        <v>79.41</v>
+      </c>
+      <c r="M8" s="4">
+        <v>66.349999999999994</v>
+      </c>
+      <c r="N8" s="4">
+        <v>63.88</v>
+      </c>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="4">
+        <v>24.62</v>
+      </c>
+      <c r="R8" s="4">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="S8" s="4">
+        <v>65.97</v>
+      </c>
+      <c r="T8" s="4">
+        <v>63.67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
@@ -1425,25 +1490,39 @@
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="J12" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="K12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="31" t="s">
+      <c r="L12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="31" t="s">
+      <c r="M12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="31" t="s">
+      <c r="N12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="30"/>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="27" t="s">
+      <c r="P12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T12" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1461,17 +1540,39 @@
       <c r="G13" s="9">
         <v>84.78</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="J13" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="30"/>
-    </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="27"/>
+      <c r="K13" s="4">
+        <v>7.99</v>
+      </c>
+      <c r="L13" s="4">
+        <v>95.24</v>
+      </c>
+      <c r="M13" s="4">
+        <v>90.84</v>
+      </c>
+      <c r="N13" s="4">
+        <v>84.77</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>9.42</v>
+      </c>
+      <c r="R13" s="4">
+        <v>93.85</v>
+      </c>
+      <c r="S13" s="4">
+        <v>89.19</v>
+      </c>
+      <c r="T13" s="4">
+        <v>83.39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1487,15 +1588,35 @@
       <c r="G14" s="9">
         <v>69.849999999999994</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="30"/>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="27"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="4">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="L14" s="4">
+        <v>92.72</v>
+      </c>
+      <c r="M14" s="4">
+        <v>88.98</v>
+      </c>
+      <c r="N14" s="4">
+        <v>82.47</v>
+      </c>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="4">
+        <v>11.31</v>
+      </c>
+      <c r="R14" s="4">
+        <v>91.51</v>
+      </c>
+      <c r="S14" s="4">
+        <v>85.35</v>
+      </c>
+      <c r="T14" s="4">
+        <v>79.34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1508,86 +1629,104 @@
       <c r="F15" s="9">
         <v>78.78</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="19">
         <v>71.38</v>
       </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="30"/>
-    </row>
-    <row r="17" spans="2:16">
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-    </row>
-    <row r="18" spans="2:16">
-      <c r="C18" s="40"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="B19" t="s">
+      <c r="J15" s="27"/>
+      <c r="K15" s="4">
+        <v>18.48</v>
+      </c>
+      <c r="L15" s="4">
+        <v>82.77</v>
+      </c>
+      <c r="M15" s="4">
+        <v>74.38</v>
+      </c>
+      <c r="N15" s="4">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="4">
+        <v>19.04</v>
+      </c>
+      <c r="R15" s="4">
+        <v>84.46</v>
+      </c>
+      <c r="S15" s="4">
+        <v>73.8</v>
+      </c>
+      <c r="T15" s="40">
+        <v>69.239999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C18" s="24"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J19" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" s="39" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16">
-      <c r="B28" s="25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16">
-      <c r="B29" t="s">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="2:16">
-      <c r="B30" t="s">
+      <c r="P20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:16">
-      <c r="B31" t="s">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
-      <c r="B37" t="s">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="26" t="s">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="26" t="s">
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="J30" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="P6:P8"/>
     <mergeCell ref="B13:B15"/>
-    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="P13:P15"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="J13:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1598,25 +1737,25 @@
   <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="M14:N14"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -1624,7 +1763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1771,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1640,7 +1779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -1657,18 +1796,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBA9A2A-1254-4B88-9610-852D86DB7252}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1706,8 +1845,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1725,27 +1864,27 @@
       <c r="G4" s="9">
         <v>84.78</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="13">
         <v>18.25</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="13">
         <v>82.24</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="13">
         <v>78.78</v>
       </c>
       <c r="N4" s="16">
         <v>71.38</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
-      <c r="B5" s="27"/>
+    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="25"/>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1761,101 +1900,101 @@
       <c r="G5" s="9">
         <v>69.849999999999994</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="36">
         <v>21.58</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="36">
         <v>81.69</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="36">
         <v>75.91</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="37">
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
-      <c r="B6" s="27"/>
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="26"/>
+      <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="13">
         <v>18.25</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="13">
         <v>82.24</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="13">
         <v>78.78</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="18">
         <v>71.38</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="36">
         <v>26</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="36">
         <v>79.19</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="36">
         <v>66.92</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="36">
         <v>62.61</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="11">
         <v>3.16</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <v>99.38</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="11">
         <v>98.62</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="11">
         <v>86.46</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="36">
         <v>23.82</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="36">
         <v>79.239999999999995</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="36">
         <v>71.510000000000005</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="36">
         <v>63.17</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="27"/>
+    <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1871,65 +2010,65 @@
       <c r="G8" s="9">
         <v>67.459999999999994</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="11">
         <v>45.59</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="11">
         <v>0</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="11">
         <v>0</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="11">
         <v>23.37</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="27"/>
-      <c r="C9" s="4" t="s">
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="26"/>
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="13">
         <v>21.58</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="13">
         <v>81.69</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="13">
         <v>75.91</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="18">
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="11">
         <v>9.5399999999999991</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="11">
         <v>95.75</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="11">
         <v>85.81</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="11">
         <v>80.44</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="27"/>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="25"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1946,46 +2085,46 @@
         <v>63.71</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="27"/>
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="26"/>
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="13">
         <v>26</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="13">
         <v>79.19</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="13">
         <v>66.92</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="13">
         <v>62.61</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="11">
         <v>2.86</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="11">
         <v>99.32</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="11">
         <v>97.86</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="11">
         <v>86.06</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="27"/>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2002,74 +2141,46 @@
         <v>66.23</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="27"/>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="26"/>
+      <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="13">
         <v>23.82</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="13">
         <v>79.239999999999995</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="13">
         <v>71.510000000000005</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="13">
         <v>63.17</v>
       </c>
-      <c r="J15" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="N15" s="22"/>
-    </row>
-    <row r="16" spans="2:14">
+    </row>
+    <row r="16" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="11">
         <v>46.21</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="11">
         <v>0</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="11">
         <v>23.58</v>
       </c>
-      <c r="J16" s="23">
-        <v>0</v>
-      </c>
-      <c r="K16" s="24">
-        <v>6.74</v>
-      </c>
-      <c r="L16" s="24">
-        <v>96.42</v>
-      </c>
-      <c r="M16" s="24">
-        <v>93.12</v>
-      </c>
-      <c r="N16" s="24">
-        <v>86.61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="B17" s="27"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2085,24 +2196,9 @@
       <c r="G17" s="9">
         <v>23.64</v>
       </c>
-      <c r="J17" s="23">
-        <v>1</v>
-      </c>
-      <c r="K17" s="24">
-        <v>20.29</v>
-      </c>
-      <c r="L17" s="24">
-        <v>82.05</v>
-      </c>
-      <c r="M17" s="24">
-        <v>73.28</v>
-      </c>
-      <c r="N17" s="24">
-        <v>67.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="B18" s="27"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="25"/>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2118,29 +2214,14 @@
       <c r="G18" s="9">
         <v>23.37</v>
       </c>
-      <c r="J18" s="23">
-        <v>2</v>
-      </c>
-      <c r="K18" s="24">
-        <v>19.72</v>
-      </c>
-      <c r="L18" s="24">
-        <v>81.25</v>
-      </c>
-      <c r="M18" s="24">
-        <v>74.569999999999993</v>
-      </c>
-      <c r="N18" s="24">
-        <v>66.02</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1"/>
-    <row r="24" spans="1:14">
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -2148,7 +2229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2257,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2187,12 +2268,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2215,7 +2296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2238,7 +2319,7 @@
         <v>77.33</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2342,7 @@
         <v>65.510000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2284,12 +2365,12 @@
         <v>63.24</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2312,7 +2393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2335,7 +2416,7 @@
         <v>84.78</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2352,7 +2433,7 @@
         <v>69.849999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2382,7 +2463,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2393,12 +2474,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2421,7 +2502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2444,7 +2525,7 @@
         <v>84.84</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2467,7 +2548,7 @@
         <v>65.08</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2490,12 +2571,12 @@
         <v>64.31</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2541,7 +2622,7 @@
         <v>86.46</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2558,7 +2639,7 @@
         <v>67.459999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2588,7 +2669,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2599,12 +2680,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2627,7 +2708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2754,7 @@
         <v>47.51</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2696,12 +2777,12 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2724,7 +2805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2747,7 +2828,7 @@
         <v>80.44</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2764,7 +2845,7 @@
         <v>63.71</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2794,7 +2875,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -2805,12 +2886,12 @@
     <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2833,7 +2914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2848,7 +2929,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2944,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2878,12 +2959,12 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2906,7 +2987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2921,7 +3002,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +3011,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2952,14 +3033,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2982,7 +3063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3005,7 +3086,7 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3028,7 +3109,7 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -3051,12 +3132,12 @@
         <v>61.09</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +3160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -3102,7 +3183,7 @@
         <v>86.06</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -3119,7 +3200,7 @@
         <v>66.23</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -3149,7 +3230,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
@@ -3160,12 +3241,12 @@
     <col min="8" max="8" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3188,7 +3269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3211,7 +3292,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3234,7 +3315,7 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -3257,12 +3338,12 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -3285,7 +3366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -3308,7 +3389,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
@@ -3325,7 +3406,7 @@
         <v>23.64</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
@@ -3352,44 +3433,35 @@
   <dimension ref="B2:U39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="5.44140625" customWidth="1"/>
     <col min="14" max="14" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-    </row>
-    <row r="5" spans="2:19">
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -3408,40 +3480,39 @@
       <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="36" t="s">
+      <c r="Q5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:19">
-      <c r="B6" s="27" t="s">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -3459,40 +3530,39 @@
       <c r="G6" s="9">
         <v>77.33</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="4">
         <v>14.57</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="4">
         <v>91.95</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="4">
         <v>80.61</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="4">
         <v>78.56</v>
       </c>
-      <c r="N6" s="30"/>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="36">
+      <c r="P6" s="23">
         <v>13.68</v>
       </c>
-      <c r="Q6" s="36">
+      <c r="Q6" s="23">
         <v>92.48</v>
       </c>
-      <c r="R6" s="36">
+      <c r="R6" s="23">
         <v>80.22</v>
       </c>
-      <c r="S6" s="36">
+      <c r="S6" s="23">
         <v>78.92</v>
       </c>
     </row>
-    <row r="7" spans="2:19">
-      <c r="B7" s="27"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -3508,36 +3578,35 @@
       <c r="G7" s="9">
         <v>65.510000000000005</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="33">
+      <c r="I7" s="32"/>
+      <c r="J7" s="4">
         <v>16</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="4">
         <v>89.81</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="4">
         <v>77.540000000000006</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="4">
         <v>77.319999999999993</v>
       </c>
-      <c r="N7" s="30"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="36">
+      <c r="O7" s="29"/>
+      <c r="P7" s="23">
         <v>23.93</v>
       </c>
-      <c r="Q7" s="36">
+      <c r="Q7" s="23">
         <v>80.989999999999995</v>
       </c>
-      <c r="R7" s="36">
+      <c r="R7" s="23">
         <v>62.6</v>
       </c>
-      <c r="S7" s="36">
+      <c r="S7" s="23">
         <v>62.04</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="15" thickBot="1">
-      <c r="B8" s="28"/>
+    <row r="8" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="26"/>
       <c r="C8" s="12" t="s">
         <v>9</v>
       </c>
@@ -3553,77 +3622,40 @@
       <c r="G8" s="13">
         <v>63.24</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="33">
+      <c r="I8" s="27"/>
+      <c r="J8" s="4">
         <v>23.11</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="4">
         <v>79.41</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="4">
         <v>66.349999999999994</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="4">
         <v>63.88</v>
       </c>
-      <c r="N8" s="30"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="36">
+      <c r="O8" s="30"/>
+      <c r="P8" s="23">
         <v>24.93</v>
       </c>
-      <c r="Q8" s="36">
+      <c r="Q8" s="23">
         <v>79.62</v>
       </c>
-      <c r="R8" s="36">
+      <c r="R8" s="23">
         <v>63.48</v>
       </c>
-      <c r="S8" s="36">
+      <c r="S8" s="23">
         <v>60.24</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="15" thickTop="1">
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" spans="2:19">
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-    </row>
-    <row r="11" spans="2:19">
+    <row r="9" spans="2:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-    </row>
-    <row r="12" spans="2:19">
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
@@ -3642,40 +3674,39 @@
       <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="31" t="s">
+      <c r="K12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="31" t="s">
+      <c r="M12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="30"/>
-      <c r="O12" s="36" t="s">
+      <c r="O12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P12" s="36" t="s">
+      <c r="P12" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="Q12" s="36" t="s">
+      <c r="Q12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="R12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="36" t="s">
+      <c r="S12" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:19">
-      <c r="B13" s="27" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -3693,40 +3724,39 @@
       <c r="G13" s="9">
         <v>84.78</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="4">
         <v>7.99</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="4">
         <v>95.24</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="4">
         <v>90.84</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="4">
         <v>84.77</v>
       </c>
-      <c r="N13" s="30"/>
-      <c r="O13" s="37" t="s">
+      <c r="O13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="36">
+      <c r="P13" s="23">
         <v>6.74</v>
       </c>
-      <c r="Q13" s="36">
+      <c r="Q13" s="23">
         <v>96.42</v>
       </c>
-      <c r="R13" s="36">
+      <c r="R13" s="23">
         <v>93.12</v>
       </c>
-      <c r="S13" s="36">
+      <c r="S13" s="23">
         <v>86.61</v>
       </c>
     </row>
-    <row r="14" spans="2:19">
-      <c r="B14" s="27"/>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -3742,36 +3772,35 @@
       <c r="G14" s="9">
         <v>69.849999999999994</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="33">
+      <c r="I14" s="32"/>
+      <c r="J14" s="4">
         <v>9.6199999999999992</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="4">
         <v>92.72</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="4">
         <v>88.98</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="4">
         <v>82.47</v>
       </c>
-      <c r="N14" s="30"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="36">
+      <c r="O14" s="29"/>
+      <c r="P14" s="23">
         <v>20.29</v>
       </c>
-      <c r="Q14" s="36">
+      <c r="Q14" s="23">
         <v>82.05</v>
       </c>
-      <c r="R14" s="36">
+      <c r="R14" s="23">
         <v>73.28</v>
       </c>
-      <c r="S14" s="36">
+      <c r="S14" s="23">
         <v>67.25</v>
       </c>
     </row>
-    <row r="15" spans="2:19">
-      <c r="B15" s="27"/>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -3784,92 +3813,91 @@
       <c r="F15" s="9">
         <v>78.78</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="19">
         <v>71.38</v>
       </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="33">
+      <c r="I15" s="27"/>
+      <c r="J15" s="4">
         <v>18.48</v>
       </c>
-      <c r="K15" s="33">
+      <c r="K15" s="4">
         <v>82.77</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="4">
         <v>74.38</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="4">
         <v>68.599999999999994</v>
       </c>
-      <c r="N15" s="30"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="36">
+      <c r="O15" s="30"/>
+      <c r="P15" s="23">
         <v>19.72</v>
       </c>
-      <c r="Q15" s="36">
+      <c r="Q15" s="23">
         <v>81.25</v>
       </c>
-      <c r="R15" s="36">
+      <c r="R15" s="23">
         <v>74.569999999999993</v>
       </c>
-      <c r="S15" s="36">
+      <c r="S15" s="23">
         <v>66.02</v>
       </c>
     </row>
-    <row r="17" spans="2:21">
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-    </row>
-    <row r="18" spans="2:21">
-      <c r="C18" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-    </row>
-    <row r="28" spans="2:21">
-      <c r="B28" s="25" t="s">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C18" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B28" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:21">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:21">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="26" t="s">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="26" t="s">
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>